<commit_message>
manga v(2.4.0.0) Gradle 'createExe' task + Command line argument support
- We include the Launch4j into Gradle. No need to make Jar any more, just we can type 'gradle createExe' andy changing the value of mainClass parameter.

- JSAP is also included to manage the command line arguments. now you can run the client passing its arguments on the command line like this:
$ equiz-client.exe -h localhost --port 10000 -u "sami fattani" -i MBA001

- Blank field now can be also used as Essay. I change the textField into textArea. It works fine.
</commit_message>
<xml_diff>
--- a/data/IT100-2-backup.xlsx
+++ b/data/IT100-2-backup.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
     <sheet name="Questions" sheetId="3" r:id="rId2"/>
     <sheet name="BlackWhite List" sheetId="4" r:id="rId3"/>
-    <sheet name="Answers" sheetId="7" r:id="rId4"/>
-    <sheet name="Timer" sheetId="8" r:id="rId5"/>
+    <sheet name="Answers" sheetId="5" r:id="rId4"/>
+    <sheet name="Timer" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="91">
   <si>
     <t>sharing folder</t>
   </si>
@@ -204,6 +204,30 @@
     <t>filter.png</t>
   </si>
   <si>
+    <t>Course ID</t>
+  </si>
+  <si>
+    <t>IT100</t>
+  </si>
+  <si>
+    <t>Course Name</t>
+  </si>
+  <si>
+    <t>Computer Skills</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
     <t>Order</t>
   </si>
   <si>
@@ -228,70 +252,49 @@
     <t>Q6</t>
   </si>
   <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 5, 6, 1</t>
+  </si>
+  <si>
+    <t>Q1/1/CBDAE/C</t>
+  </si>
+  <si>
+    <t>Q2/1/BEDCA/E</t>
+  </si>
+  <si>
+    <t>Q3/1/a</t>
+  </si>
+  <si>
+    <t>Q4/1/EABCDF/A</t>
+  </si>
+  <si>
+    <t>Q5/1/ADBC/B</t>
+  </si>
+  <si>
+    <t>Q6/1/AB/A</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>00:01</t>
-  </si>
-  <si>
-    <t>00:03</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Q2/1/AECBD/A</t>
-  </si>
-  <si>
-    <t>Q4/1/DACEB/A</t>
-  </si>
-  <si>
-    <t>Q5/1/DACB/A</t>
-  </si>
-  <si>
     <t>00:02</t>
   </si>
   <si>
-    <t>04:45</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 4, 5, 6</t>
-  </si>
-  <si>
-    <t>Q3/1/A</t>
-  </si>
-  <si>
-    <t>Course ID</t>
-  </si>
-  <si>
-    <t>IT100</t>
-  </si>
-  <si>
-    <t>Course Name</t>
-  </si>
-  <si>
-    <t>Computer Skills</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Semester</t>
-  </si>
-  <si>
-    <t>Fall</t>
-  </si>
-  <si>
-    <t>Q6/AB/1/B</t>
-  </si>
-  <si>
-    <t>Q1/1/ECBDA/B</t>
+    <t>00:06</t>
+  </si>
+  <si>
+    <t>00:08</t>
+  </si>
+  <si>
+    <t>00:04</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>2nd MidTerm</t>
   </si>
 </sst>
 </file>
@@ -894,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B7:B8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -976,23 +979,23 @@
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="30" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="30" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B9" s="32">
         <v>1</v>
@@ -1000,7 +1003,7 @@
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="30" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B10" s="32">
         <v>2016</v>
@@ -1008,10 +1011,18 @@
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="30" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>87</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1046,7 +1057,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1389,26 +1400,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="2.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1420,97 +1429,97 @@
         <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="J1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="L1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="M1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="N1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="O1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2">
         <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>88</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
       </c>
       <c r="P2">
         <f>SUMIF(D2:O2,  "&gt;0")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1520,11 +1529,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1542,54 +1549,54 @@
         <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="H1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>76</v>
       </c>
-      <c r="D3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3">
-        <f>SUM(C3:H3)</f>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2">
+        <f>SUM(C2:H2)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>